<commit_message>
slight change and no need for just csv
</commit_message>
<xml_diff>
--- a/Outputs/reconstructedWGFPDailyFlow.xlsx
+++ b/Outputs/reconstructedWGFPDailyFlow.xlsx
@@ -396,8 +396,8 @@
       <c r="B3" t="inlineStr">
         <is>
           <t xml:space="preserve">Used available data from gage FRAGRACO provided by Northern water to CDSS https://dwr.state.co.us/Tools/Stations/FRAGRACO. For data gaps, 
-          assumed Fraser Flow was calculated by subtracting 'Assumed/Actual Upper C Flow' from 'CR Below WG Flow' + 
-          'Windy gap pumping flow' (https://dwr.state.co.us/Tools/Stations/WGPPMPCO) </t>
+          assumed Fraser Flow was calculated by subtracting 'Assumed/Actual Upper C Flow' from 'CR Below WG Flow' + 'Windy gap pumping flow' (https://dwr.state.co.us/Tools/Stations/WGPPMPCO). 
+          No correction factor was used due to inconsistent pumping flows out of Windy Gap. </t>
         </is>
       </c>
     </row>

</xml_diff>